<commit_message>
Working on website utility
</commit_message>
<xml_diff>
--- a/livingdex.xlsx
+++ b/livingdex.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3091" uniqueCount="1046">
   <si>
     <t>#</t>
   </si>
@@ -2582,6 +2582,22 @@
   </si>
   <si>
     <t>Boltund</t>
+  </si>
+  <si>
+    <t>Brilliant Stars
+#TG13</t>
+  </si>
+  <si>
+    <t>Sword &amp; Shield Promos
+#SWSH219</t>
+  </si>
+  <si>
+    <t>Temporal Forces
+#59</t>
+  </si>
+  <si>
+    <t>Battle Styles
+#53</t>
   </si>
   <si>
     <t>Rolycoly</t>
@@ -20357,13 +20373,34 @@
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/836/1.png", 2)</f>
         <v>0</v>
       </c>
+      <c r="D2507">
+        <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/836/2.png", 2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2507">
+        <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/836/3.png", 2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2507">
+        <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/836/4.png", 2)</f>
+        <v>0</v>
+      </c>
       <c r="G2507" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2508" spans="1:7">
       <c r="C2508" s="4" t="s">
-        <v>20</v>
+        <v>853</v>
+      </c>
+      <c r="D2508" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="E2508" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="F2508" s="4" t="s">
+        <v>856</v>
       </c>
     </row>
     <row r="2510" spans="1:7" ht="264" customHeight="1">
@@ -20371,7 +20408,7 @@
         <v>837</v>
       </c>
       <c r="B2510" s="3" t="s">
-        <v>853</v>
+        <v>857</v>
       </c>
       <c r="C2510">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/837/1.png", 2)</f>
@@ -20391,7 +20428,7 @@
         <v>838</v>
       </c>
       <c r="B2513" s="3" t="s">
-        <v>854</v>
+        <v>858</v>
       </c>
       <c r="C2513">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/838/1.png", 2)</f>
@@ -20411,7 +20448,7 @@
         <v>839</v>
       </c>
       <c r="B2516" s="3" t="s">
-        <v>855</v>
+        <v>859</v>
       </c>
       <c r="C2516">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/839/1.png", 2)</f>
@@ -20431,7 +20468,7 @@
         <v>840</v>
       </c>
       <c r="B2519" s="3" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="C2519">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/840/1.png", 2)</f>
@@ -20451,7 +20488,7 @@
         <v>841</v>
       </c>
       <c r="B2522" s="3" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="C2522">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/841/1.png", 2)</f>
@@ -20471,7 +20508,7 @@
         <v>842</v>
       </c>
       <c r="B2525" s="3" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="C2525">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/842/1.png", 2)</f>
@@ -20491,7 +20528,7 @@
         <v>843</v>
       </c>
       <c r="B2528" s="3" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="C2528">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/843/1.png", 2)</f>
@@ -20511,7 +20548,7 @@
         <v>844</v>
       </c>
       <c r="B2531" s="3" t="s">
-        <v>860</v>
+        <v>864</v>
       </c>
       <c r="C2531">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/844/1.png", 2)</f>
@@ -20531,7 +20568,7 @@
         <v>845</v>
       </c>
       <c r="B2534" s="3" t="s">
-        <v>861</v>
+        <v>865</v>
       </c>
       <c r="C2534">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/845/1.png", 2)</f>
@@ -20551,7 +20588,7 @@
         <v>846</v>
       </c>
       <c r="B2537" s="3" t="s">
-        <v>862</v>
+        <v>866</v>
       </c>
       <c r="C2537">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/846/1.png", 2)</f>
@@ -20571,7 +20608,7 @@
         <v>847</v>
       </c>
       <c r="B2540" s="3" t="s">
-        <v>863</v>
+        <v>867</v>
       </c>
       <c r="C2540">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/847/1.png", 2)</f>
@@ -20591,7 +20628,7 @@
         <v>848</v>
       </c>
       <c r="B2543" s="3" t="s">
-        <v>864</v>
+        <v>868</v>
       </c>
       <c r="C2543">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/848/1.png", 2)</f>
@@ -20611,7 +20648,7 @@
         <v>849</v>
       </c>
       <c r="B2546" s="3" t="s">
-        <v>865</v>
+        <v>869</v>
       </c>
       <c r="C2546">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/849/1.png", 2)</f>
@@ -20631,7 +20668,7 @@
         <v>850</v>
       </c>
       <c r="B2549" s="3" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="C2549">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/850/1.png", 2)</f>
@@ -20651,7 +20688,7 @@
         <v>851</v>
       </c>
       <c r="B2552" s="3" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="C2552">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/851/1.png", 2)</f>
@@ -20671,7 +20708,7 @@
         <v>852</v>
       </c>
       <c r="B2555" s="3" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="C2555">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/852/1.png", 2)</f>
@@ -20691,7 +20728,7 @@
         <v>853</v>
       </c>
       <c r="B2558" s="3" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="C2558">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/853/1.png", 2)</f>
@@ -20711,7 +20748,7 @@
         <v>854</v>
       </c>
       <c r="B2561" s="3" t="s">
-        <v>870</v>
+        <v>874</v>
       </c>
       <c r="C2561">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/854/1.png", 2)</f>
@@ -20731,7 +20768,7 @@
         <v>855</v>
       </c>
       <c r="B2564" s="3" t="s">
-        <v>871</v>
+        <v>875</v>
       </c>
       <c r="C2564">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/855/1.png", 2)</f>
@@ -20751,7 +20788,7 @@
         <v>856</v>
       </c>
       <c r="B2567" s="3" t="s">
-        <v>872</v>
+        <v>876</v>
       </c>
       <c r="C2567">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/856/1.png", 2)</f>
@@ -20771,7 +20808,7 @@
         <v>857</v>
       </c>
       <c r="B2570" s="3" t="s">
-        <v>873</v>
+        <v>877</v>
       </c>
       <c r="C2570">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/857/1.png", 2)</f>
@@ -20791,7 +20828,7 @@
         <v>858</v>
       </c>
       <c r="B2573" s="3" t="s">
-        <v>874</v>
+        <v>878</v>
       </c>
       <c r="C2573">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/858/1.png", 2)</f>
@@ -20811,7 +20848,7 @@
         <v>859</v>
       </c>
       <c r="B2576" s="3" t="s">
-        <v>875</v>
+        <v>879</v>
       </c>
       <c r="C2576">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/859/1.png", 2)</f>
@@ -20831,7 +20868,7 @@
         <v>860</v>
       </c>
       <c r="B2579" s="3" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="C2579">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/860/1.png", 2)</f>
@@ -20851,7 +20888,7 @@
         <v>861</v>
       </c>
       <c r="B2582" s="3" t="s">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="C2582">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/861/1.png", 2)</f>
@@ -20871,7 +20908,7 @@
         <v>862</v>
       </c>
       <c r="B2585" s="3" t="s">
-        <v>878</v>
+        <v>882</v>
       </c>
       <c r="C2585">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/862/1.png", 2)</f>
@@ -20891,7 +20928,7 @@
         <v>863</v>
       </c>
       <c r="B2588" s="3" t="s">
-        <v>879</v>
+        <v>883</v>
       </c>
       <c r="C2588">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/863/1.png", 2)</f>
@@ -20911,7 +20948,7 @@
         <v>864</v>
       </c>
       <c r="B2591" s="3" t="s">
-        <v>880</v>
+        <v>884</v>
       </c>
       <c r="C2591">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/864/1.png", 2)</f>
@@ -20931,7 +20968,7 @@
         <v>865</v>
       </c>
       <c r="B2594" s="3" t="s">
-        <v>881</v>
+        <v>885</v>
       </c>
       <c r="C2594">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/865/1.png", 2)</f>
@@ -20951,7 +20988,7 @@
         <v>866</v>
       </c>
       <c r="B2597" s="3" t="s">
-        <v>882</v>
+        <v>886</v>
       </c>
       <c r="C2597">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/866/1.png", 2)</f>
@@ -20971,7 +21008,7 @@
         <v>867</v>
       </c>
       <c r="B2600" s="3" t="s">
-        <v>883</v>
+        <v>887</v>
       </c>
       <c r="C2600">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/867/1.png", 2)</f>
@@ -20991,7 +21028,7 @@
         <v>868</v>
       </c>
       <c r="B2603" s="3" t="s">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="C2603">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/868/1.png", 2)</f>
@@ -21011,7 +21048,7 @@
         <v>869</v>
       </c>
       <c r="B2606" s="3" t="s">
-        <v>885</v>
+        <v>889</v>
       </c>
       <c r="C2606">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/869/1.png", 2)</f>
@@ -21031,7 +21068,7 @@
         <v>870</v>
       </c>
       <c r="B2609" s="3" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="C2609">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/870/1.png", 2)</f>
@@ -21051,7 +21088,7 @@
         <v>871</v>
       </c>
       <c r="B2612" s="3" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
       <c r="C2612">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/871/1.png", 2)</f>
@@ -21071,7 +21108,7 @@
         <v>872</v>
       </c>
       <c r="B2615" s="3" t="s">
-        <v>888</v>
+        <v>892</v>
       </c>
       <c r="C2615">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/872/1.png", 2)</f>
@@ -21091,7 +21128,7 @@
         <v>873</v>
       </c>
       <c r="B2618" s="3" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="C2618">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/873/1.png", 2)</f>
@@ -21111,7 +21148,7 @@
         <v>874</v>
       </c>
       <c r="B2621" s="3" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="C2621">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/874/1.png", 2)</f>
@@ -21131,7 +21168,7 @@
         <v>875</v>
       </c>
       <c r="B2624" s="3" t="s">
-        <v>891</v>
+        <v>895</v>
       </c>
       <c r="C2624">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/875/1.png", 2)</f>
@@ -21151,7 +21188,7 @@
         <v>876</v>
       </c>
       <c r="B2627" s="3" t="s">
-        <v>892</v>
+        <v>896</v>
       </c>
       <c r="C2627">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/876/1.png", 2)</f>
@@ -21171,7 +21208,7 @@
         <v>877</v>
       </c>
       <c r="B2630" s="3" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
       <c r="C2630">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/877/1.png", 2)</f>
@@ -21191,7 +21228,7 @@
         <v>878</v>
       </c>
       <c r="B2633" s="3" t="s">
-        <v>894</v>
+        <v>898</v>
       </c>
       <c r="C2633">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/878/1.png", 2)</f>
@@ -21211,7 +21248,7 @@
         <v>879</v>
       </c>
       <c r="B2636" s="3" t="s">
-        <v>895</v>
+        <v>899</v>
       </c>
       <c r="C2636">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/879/1.png", 2)</f>
@@ -21231,7 +21268,7 @@
         <v>880</v>
       </c>
       <c r="B2639" s="3" t="s">
-        <v>896</v>
+        <v>900</v>
       </c>
       <c r="C2639">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/880/1.png", 2)</f>
@@ -21251,7 +21288,7 @@
         <v>881</v>
       </c>
       <c r="B2642" s="3" t="s">
-        <v>897</v>
+        <v>901</v>
       </c>
       <c r="C2642">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/881/1.png", 2)</f>
@@ -21271,7 +21308,7 @@
         <v>882</v>
       </c>
       <c r="B2645" s="3" t="s">
-        <v>898</v>
+        <v>902</v>
       </c>
       <c r="C2645">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/882/1.png", 2)</f>
@@ -21291,7 +21328,7 @@
         <v>883</v>
       </c>
       <c r="B2648" s="3" t="s">
-        <v>899</v>
+        <v>903</v>
       </c>
       <c r="C2648">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/883/1.png", 2)</f>
@@ -21311,7 +21348,7 @@
         <v>884</v>
       </c>
       <c r="B2651" s="3" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="C2651">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/884/1.png", 2)</f>
@@ -21331,7 +21368,7 @@
         <v>885</v>
       </c>
       <c r="B2654" s="3" t="s">
-        <v>901</v>
+        <v>905</v>
       </c>
       <c r="C2654">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/885/1.png", 2)</f>
@@ -21351,7 +21388,7 @@
         <v>886</v>
       </c>
       <c r="B2657" s="3" t="s">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c r="C2657">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/886/1.png", 2)</f>
@@ -21371,7 +21408,7 @@
         <v>887</v>
       </c>
       <c r="B2660" s="3" t="s">
-        <v>903</v>
+        <v>907</v>
       </c>
       <c r="C2660">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/887/1.png", 2)</f>
@@ -21391,7 +21428,7 @@
         <v>888</v>
       </c>
       <c r="B2663" s="3" t="s">
-        <v>904</v>
+        <v>908</v>
       </c>
       <c r="C2663">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/888/1.png", 2)</f>
@@ -21411,7 +21448,7 @@
         <v>889</v>
       </c>
       <c r="B2666" s="3" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c r="C2666">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/889/1.png", 2)</f>
@@ -21431,7 +21468,7 @@
         <v>890</v>
       </c>
       <c r="B2669" s="3" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
       <c r="C2669">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/890/1.png", 2)</f>
@@ -21451,7 +21488,7 @@
         <v>891</v>
       </c>
       <c r="B2672" s="3" t="s">
-        <v>907</v>
+        <v>911</v>
       </c>
       <c r="C2672">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/891/1.png", 2)</f>
@@ -21471,7 +21508,7 @@
         <v>892</v>
       </c>
       <c r="B2675" s="3" t="s">
-        <v>908</v>
+        <v>912</v>
       </c>
       <c r="C2675">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/892/1.png", 2)</f>
@@ -21491,7 +21528,7 @@
         <v>893</v>
       </c>
       <c r="B2678" s="3" t="s">
-        <v>909</v>
+        <v>913</v>
       </c>
       <c r="C2678">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/893/1.png", 2)</f>
@@ -21511,7 +21548,7 @@
         <v>894</v>
       </c>
       <c r="B2681" s="3" t="s">
-        <v>910</v>
+        <v>914</v>
       </c>
       <c r="C2681">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/894/1.png", 2)</f>
@@ -21531,7 +21568,7 @@
         <v>895</v>
       </c>
       <c r="B2684" s="3" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="C2684">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/895/1.png", 2)</f>
@@ -21551,7 +21588,7 @@
         <v>896</v>
       </c>
       <c r="B2687" s="3" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="C2687">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/896/1.png", 2)</f>
@@ -21571,7 +21608,7 @@
         <v>897</v>
       </c>
       <c r="B2690" s="3" t="s">
-        <v>913</v>
+        <v>917</v>
       </c>
       <c r="C2690">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/897/1.png", 2)</f>
@@ -21591,7 +21628,7 @@
         <v>898</v>
       </c>
       <c r="B2693" s="3" t="s">
-        <v>914</v>
+        <v>918</v>
       </c>
       <c r="C2693">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/898/1.png", 2)</f>
@@ -21611,7 +21648,7 @@
         <v>899</v>
       </c>
       <c r="B2696" s="3" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="C2696">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/899/1.png", 2)</f>
@@ -21631,7 +21668,7 @@
         <v>900</v>
       </c>
       <c r="B2699" s="3" t="s">
-        <v>916</v>
+        <v>920</v>
       </c>
       <c r="C2699">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/900/1.png", 2)</f>
@@ -21651,7 +21688,7 @@
         <v>901</v>
       </c>
       <c r="B2702" s="3" t="s">
-        <v>917</v>
+        <v>921</v>
       </c>
       <c r="C2702">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/901/1.png", 2)</f>
@@ -21671,7 +21708,7 @@
         <v>902</v>
       </c>
       <c r="B2705" s="3" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="C2705">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/902/1.png", 2)</f>
@@ -21691,7 +21728,7 @@
         <v>903</v>
       </c>
       <c r="B2708" s="3" t="s">
-        <v>919</v>
+        <v>923</v>
       </c>
       <c r="C2708">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/903/1.png", 2)</f>
@@ -21711,7 +21748,7 @@
         <v>904</v>
       </c>
       <c r="B2711" s="3" t="s">
-        <v>920</v>
+        <v>924</v>
       </c>
       <c r="C2711">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/904/1.png", 2)</f>
@@ -21731,7 +21768,7 @@
         <v>905</v>
       </c>
       <c r="B2714" s="3" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="C2714">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/905/1.png", 2)</f>
@@ -21751,7 +21788,7 @@
         <v>906</v>
       </c>
       <c r="B2717" s="3" t="s">
-        <v>922</v>
+        <v>926</v>
       </c>
       <c r="C2717">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/906/1.png", 2)</f>
@@ -21771,7 +21808,7 @@
         <v>907</v>
       </c>
       <c r="B2720" s="3" t="s">
-        <v>923</v>
+        <v>927</v>
       </c>
       <c r="C2720">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/907/1.png", 2)</f>
@@ -21791,7 +21828,7 @@
         <v>908</v>
       </c>
       <c r="B2723" s="3" t="s">
-        <v>924</v>
+        <v>928</v>
       </c>
       <c r="C2723">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/908/1.png", 2)</f>
@@ -21811,7 +21848,7 @@
         <v>909</v>
       </c>
       <c r="B2726" s="3" t="s">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="C2726">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/909/1.png", 2)</f>
@@ -21831,7 +21868,7 @@
         <v>910</v>
       </c>
       <c r="B2729" s="3" t="s">
-        <v>926</v>
+        <v>930</v>
       </c>
       <c r="C2729">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/910/1.png", 2)</f>
@@ -21851,7 +21888,7 @@
         <v>911</v>
       </c>
       <c r="B2732" s="3" t="s">
-        <v>927</v>
+        <v>931</v>
       </c>
       <c r="C2732">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/911/1.png", 2)</f>
@@ -21871,7 +21908,7 @@
         <v>912</v>
       </c>
       <c r="B2735" s="3" t="s">
-        <v>928</v>
+        <v>932</v>
       </c>
       <c r="C2735">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/912/1.png", 2)</f>
@@ -21891,7 +21928,7 @@
         <v>913</v>
       </c>
       <c r="B2738" s="3" t="s">
-        <v>929</v>
+        <v>933</v>
       </c>
       <c r="C2738">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/913/1.png", 2)</f>
@@ -21911,7 +21948,7 @@
         <v>914</v>
       </c>
       <c r="B2741" s="3" t="s">
-        <v>930</v>
+        <v>934</v>
       </c>
       <c r="C2741">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/914/1.png", 2)</f>
@@ -21931,7 +21968,7 @@
         <v>915</v>
       </c>
       <c r="B2744" s="3" t="s">
-        <v>931</v>
+        <v>935</v>
       </c>
       <c r="C2744">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/915/1.png", 2)</f>
@@ -21951,7 +21988,7 @@
         <v>916</v>
       </c>
       <c r="B2747" s="3" t="s">
-        <v>932</v>
+        <v>936</v>
       </c>
       <c r="C2747">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/916/1.png", 2)</f>
@@ -21971,7 +22008,7 @@
         <v>917</v>
       </c>
       <c r="B2750" s="3" t="s">
-        <v>933</v>
+        <v>937</v>
       </c>
       <c r="C2750">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/917/1.png", 2)</f>
@@ -21991,7 +22028,7 @@
         <v>918</v>
       </c>
       <c r="B2753" s="3" t="s">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="C2753">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/918/1.png", 2)</f>
@@ -22011,7 +22048,7 @@
         <v>919</v>
       </c>
       <c r="B2756" s="3" t="s">
-        <v>935</v>
+        <v>939</v>
       </c>
       <c r="C2756">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/919/1.png", 2)</f>
@@ -22031,7 +22068,7 @@
         <v>920</v>
       </c>
       <c r="B2759" s="3" t="s">
-        <v>936</v>
+        <v>940</v>
       </c>
       <c r="C2759">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/920/1.png", 2)</f>
@@ -22051,7 +22088,7 @@
         <v>921</v>
       </c>
       <c r="B2762" s="3" t="s">
-        <v>937</v>
+        <v>941</v>
       </c>
       <c r="C2762">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/921/1.png", 2)</f>
@@ -22071,7 +22108,7 @@
         <v>922</v>
       </c>
       <c r="B2765" s="3" t="s">
-        <v>938</v>
+        <v>942</v>
       </c>
       <c r="C2765">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/922/1.png", 2)</f>
@@ -22091,7 +22128,7 @@
         <v>923</v>
       </c>
       <c r="B2768" s="3" t="s">
-        <v>939</v>
+        <v>943</v>
       </c>
       <c r="C2768">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/923/1.png", 2)</f>
@@ -22111,7 +22148,7 @@
         <v>924</v>
       </c>
       <c r="B2771" s="3" t="s">
-        <v>940</v>
+        <v>944</v>
       </c>
       <c r="C2771">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/924/1.png", 2)</f>
@@ -22131,7 +22168,7 @@
         <v>925</v>
       </c>
       <c r="B2774" s="3" t="s">
-        <v>941</v>
+        <v>945</v>
       </c>
       <c r="C2774">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/925/1.png", 2)</f>
@@ -22151,7 +22188,7 @@
         <v>926</v>
       </c>
       <c r="B2777" s="3" t="s">
-        <v>942</v>
+        <v>946</v>
       </c>
       <c r="C2777">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/926/1.png", 2)</f>
@@ -22171,7 +22208,7 @@
         <v>927</v>
       </c>
       <c r="B2780" s="3" t="s">
-        <v>943</v>
+        <v>947</v>
       </c>
       <c r="C2780">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/927/1.png", 2)</f>
@@ -22191,7 +22228,7 @@
         <v>928</v>
       </c>
       <c r="B2783" s="3" t="s">
-        <v>944</v>
+        <v>948</v>
       </c>
       <c r="C2783">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/928/1.png", 2)</f>
@@ -22211,7 +22248,7 @@
         <v>929</v>
       </c>
       <c r="B2786" s="3" t="s">
-        <v>945</v>
+        <v>949</v>
       </c>
       <c r="C2786">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/929/1.png", 2)</f>
@@ -22231,7 +22268,7 @@
         <v>930</v>
       </c>
       <c r="B2789" s="3" t="s">
-        <v>946</v>
+        <v>950</v>
       </c>
       <c r="C2789">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/930/1.png", 2)</f>
@@ -22251,7 +22288,7 @@
         <v>931</v>
       </c>
       <c r="B2792" s="3" t="s">
-        <v>947</v>
+        <v>951</v>
       </c>
       <c r="C2792">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/931/1.png", 2)</f>
@@ -22271,7 +22308,7 @@
         <v>932</v>
       </c>
       <c r="B2795" s="3" t="s">
-        <v>948</v>
+        <v>952</v>
       </c>
       <c r="C2795">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/932/1.png", 2)</f>
@@ -22291,7 +22328,7 @@
         <v>933</v>
       </c>
       <c r="B2798" s="3" t="s">
-        <v>949</v>
+        <v>953</v>
       </c>
       <c r="C2798">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/933/1.png", 2)</f>
@@ -22311,7 +22348,7 @@
         <v>934</v>
       </c>
       <c r="B2801" s="3" t="s">
-        <v>950</v>
+        <v>954</v>
       </c>
       <c r="C2801">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/934/1.png", 2)</f>
@@ -22331,7 +22368,7 @@
         <v>935</v>
       </c>
       <c r="B2804" s="3" t="s">
-        <v>951</v>
+        <v>955</v>
       </c>
       <c r="C2804">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/935/1.png", 2)</f>
@@ -22351,7 +22388,7 @@
         <v>936</v>
       </c>
       <c r="B2807" s="3" t="s">
-        <v>952</v>
+        <v>956</v>
       </c>
       <c r="C2807">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/936/1.png", 2)</f>
@@ -22371,7 +22408,7 @@
         <v>937</v>
       </c>
       <c r="B2810" s="3" t="s">
-        <v>953</v>
+        <v>957</v>
       </c>
       <c r="C2810">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/937/1.png", 2)</f>
@@ -22391,7 +22428,7 @@
         <v>938</v>
       </c>
       <c r="B2813" s="3" t="s">
-        <v>954</v>
+        <v>958</v>
       </c>
       <c r="C2813">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/938/1.png", 2)</f>
@@ -22411,7 +22448,7 @@
         <v>939</v>
       </c>
       <c r="B2816" s="3" t="s">
-        <v>955</v>
+        <v>959</v>
       </c>
       <c r="C2816">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/939/1.png", 2)</f>
@@ -22431,7 +22468,7 @@
         <v>940</v>
       </c>
       <c r="B2819" s="3" t="s">
-        <v>956</v>
+        <v>960</v>
       </c>
       <c r="C2819">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/940/1.png", 2)</f>
@@ -22451,7 +22488,7 @@
         <v>941</v>
       </c>
       <c r="B2822" s="3" t="s">
-        <v>957</v>
+        <v>961</v>
       </c>
       <c r="C2822">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/941/1.png", 2)</f>
@@ -22471,7 +22508,7 @@
         <v>942</v>
       </c>
       <c r="B2825" s="3" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="C2825">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/942/1.png", 2)</f>
@@ -22491,7 +22528,7 @@
         <v>943</v>
       </c>
       <c r="B2828" s="3" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="C2828">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/943/1.png", 2)</f>
@@ -22511,7 +22548,7 @@
         <v>944</v>
       </c>
       <c r="B2831" s="3" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c r="C2831">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/944/1.png", 2)</f>
@@ -22531,7 +22568,7 @@
         <v>945</v>
       </c>
       <c r="B2834" s="3" t="s">
-        <v>961</v>
+        <v>965</v>
       </c>
       <c r="C2834">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/945/1.png", 2)</f>
@@ -22551,7 +22588,7 @@
         <v>946</v>
       </c>
       <c r="B2837" s="3" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="C2837">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/946/1.png", 2)</f>
@@ -22571,7 +22608,7 @@
         <v>947</v>
       </c>
       <c r="B2840" s="3" t="s">
-        <v>963</v>
+        <v>967</v>
       </c>
       <c r="C2840">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/947/1.png", 2)</f>
@@ -22591,7 +22628,7 @@
         <v>948</v>
       </c>
       <c r="B2843" s="3" t="s">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c r="C2843">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/948/1.png", 2)</f>
@@ -22611,7 +22648,7 @@
         <v>949</v>
       </c>
       <c r="B2846" s="3" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="C2846">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/949/1.png", 2)</f>
@@ -22631,7 +22668,7 @@
         <v>950</v>
       </c>
       <c r="B2849" s="3" t="s">
-        <v>966</v>
+        <v>970</v>
       </c>
       <c r="C2849">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/950/1.png", 2)</f>
@@ -22651,7 +22688,7 @@
         <v>951</v>
       </c>
       <c r="B2852" s="3" t="s">
-        <v>967</v>
+        <v>971</v>
       </c>
       <c r="C2852">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/951/1.png", 2)</f>
@@ -22671,7 +22708,7 @@
         <v>952</v>
       </c>
       <c r="B2855" s="3" t="s">
-        <v>968</v>
+        <v>972</v>
       </c>
       <c r="C2855">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/952/1.png", 2)</f>
@@ -22691,7 +22728,7 @@
         <v>953</v>
       </c>
       <c r="B2858" s="3" t="s">
-        <v>969</v>
+        <v>973</v>
       </c>
       <c r="C2858">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/953/1.png", 2)</f>
@@ -22711,7 +22748,7 @@
         <v>954</v>
       </c>
       <c r="B2861" s="3" t="s">
-        <v>970</v>
+        <v>974</v>
       </c>
       <c r="C2861">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/954/1.png", 2)</f>
@@ -22731,7 +22768,7 @@
         <v>955</v>
       </c>
       <c r="B2864" s="3" t="s">
-        <v>971</v>
+        <v>975</v>
       </c>
       <c r="C2864">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/955/1.png", 2)</f>
@@ -22751,7 +22788,7 @@
         <v>956</v>
       </c>
       <c r="B2867" s="3" t="s">
-        <v>972</v>
+        <v>976</v>
       </c>
       <c r="C2867">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/956/1.png", 2)</f>
@@ -22771,7 +22808,7 @@
         <v>957</v>
       </c>
       <c r="B2870" s="3" t="s">
-        <v>973</v>
+        <v>977</v>
       </c>
       <c r="C2870">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/957/1.png", 2)</f>
@@ -22791,7 +22828,7 @@
         <v>958</v>
       </c>
       <c r="B2873" s="3" t="s">
-        <v>974</v>
+        <v>978</v>
       </c>
       <c r="C2873">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/958/1.png", 2)</f>
@@ -22811,7 +22848,7 @@
         <v>959</v>
       </c>
       <c r="B2876" s="3" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="C2876">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/959/1.png", 2)</f>
@@ -22831,7 +22868,7 @@
         <v>960</v>
       </c>
       <c r="B2879" s="3" t="s">
-        <v>976</v>
+        <v>980</v>
       </c>
       <c r="C2879">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/960/1.png", 2)</f>
@@ -22851,7 +22888,7 @@
         <v>961</v>
       </c>
       <c r="B2882" s="3" t="s">
-        <v>977</v>
+        <v>981</v>
       </c>
       <c r="C2882">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/961/1.png", 2)</f>
@@ -22871,7 +22908,7 @@
         <v>962</v>
       </c>
       <c r="B2885" s="3" t="s">
-        <v>978</v>
+        <v>982</v>
       </c>
       <c r="C2885">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/962/1.png", 2)</f>
@@ -22891,7 +22928,7 @@
         <v>963</v>
       </c>
       <c r="B2888" s="3" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="C2888">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/963/1.png", 2)</f>
@@ -22911,7 +22948,7 @@
         <v>964</v>
       </c>
       <c r="B2891" s="3" t="s">
-        <v>980</v>
+        <v>984</v>
       </c>
       <c r="C2891">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/964/1.png", 2)</f>
@@ -22931,7 +22968,7 @@
         <v>965</v>
       </c>
       <c r="B2894" s="3" t="s">
-        <v>981</v>
+        <v>985</v>
       </c>
       <c r="C2894">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/965/1.png", 2)</f>
@@ -22951,7 +22988,7 @@
         <v>966</v>
       </c>
       <c r="B2897" s="3" t="s">
-        <v>982</v>
+        <v>986</v>
       </c>
       <c r="C2897">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/966/1.png", 2)</f>
@@ -22971,7 +23008,7 @@
         <v>967</v>
       </c>
       <c r="B2900" s="3" t="s">
-        <v>983</v>
+        <v>987</v>
       </c>
       <c r="C2900">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/967/1.png", 2)</f>
@@ -22991,7 +23028,7 @@
         <v>968</v>
       </c>
       <c r="B2903" s="3" t="s">
-        <v>984</v>
+        <v>988</v>
       </c>
       <c r="C2903">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/968/1.png", 2)</f>
@@ -23011,7 +23048,7 @@
         <v>969</v>
       </c>
       <c r="B2906" s="3" t="s">
-        <v>985</v>
+        <v>989</v>
       </c>
       <c r="C2906">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/969/1.png", 2)</f>
@@ -23031,7 +23068,7 @@
         <v>970</v>
       </c>
       <c r="B2909" s="3" t="s">
-        <v>986</v>
+        <v>990</v>
       </c>
       <c r="C2909">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/970/1.png", 2)</f>
@@ -23051,7 +23088,7 @@
         <v>971</v>
       </c>
       <c r="B2912" s="3" t="s">
-        <v>987</v>
+        <v>991</v>
       </c>
       <c r="C2912">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/971/1.png", 2)</f>
@@ -23071,7 +23108,7 @@
         <v>972</v>
       </c>
       <c r="B2915" s="3" t="s">
-        <v>988</v>
+        <v>992</v>
       </c>
       <c r="C2915">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/972/1.png", 2)</f>
@@ -23091,7 +23128,7 @@
         <v>973</v>
       </c>
       <c r="B2918" s="3" t="s">
-        <v>989</v>
+        <v>993</v>
       </c>
       <c r="C2918">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/973/1.png", 2)</f>
@@ -23111,7 +23148,7 @@
         <v>974</v>
       </c>
       <c r="B2921" s="3" t="s">
-        <v>990</v>
+        <v>994</v>
       </c>
       <c r="C2921">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/974/1.png", 2)</f>
@@ -23131,7 +23168,7 @@
         <v>975</v>
       </c>
       <c r="B2924" s="3" t="s">
-        <v>991</v>
+        <v>995</v>
       </c>
       <c r="C2924">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/975/1.png", 2)</f>
@@ -23151,7 +23188,7 @@
         <v>976</v>
       </c>
       <c r="B2927" s="3" t="s">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c r="C2927">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/976/1.png", 2)</f>
@@ -23171,7 +23208,7 @@
         <v>977</v>
       </c>
       <c r="B2930" s="3" t="s">
-        <v>993</v>
+        <v>997</v>
       </c>
       <c r="C2930">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/977/1.png", 2)</f>
@@ -23191,7 +23228,7 @@
         <v>978</v>
       </c>
       <c r="B2933" s="3" t="s">
-        <v>994</v>
+        <v>998</v>
       </c>
       <c r="C2933">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/978/1.png", 2)</f>
@@ -23211,7 +23248,7 @@
         <v>979</v>
       </c>
       <c r="B2936" s="3" t="s">
-        <v>995</v>
+        <v>999</v>
       </c>
       <c r="C2936">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/979/1.png", 2)</f>
@@ -23231,7 +23268,7 @@
         <v>980</v>
       </c>
       <c r="B2939" s="3" t="s">
-        <v>996</v>
+        <v>1000</v>
       </c>
       <c r="C2939">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/980/1.png", 2)</f>
@@ -23251,7 +23288,7 @@
         <v>981</v>
       </c>
       <c r="B2942" s="3" t="s">
-        <v>997</v>
+        <v>1001</v>
       </c>
       <c r="C2942">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/981/1.png", 2)</f>
@@ -23271,7 +23308,7 @@
         <v>982</v>
       </c>
       <c r="B2945" s="3" t="s">
-        <v>998</v>
+        <v>1002</v>
       </c>
       <c r="C2945">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/982/1.png", 2)</f>
@@ -23291,7 +23328,7 @@
         <v>983</v>
       </c>
       <c r="B2948" s="3" t="s">
-        <v>999</v>
+        <v>1003</v>
       </c>
       <c r="C2948">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/983/1.png", 2)</f>
@@ -23311,7 +23348,7 @@
         <v>984</v>
       </c>
       <c r="B2951" s="3" t="s">
-        <v>1000</v>
+        <v>1004</v>
       </c>
       <c r="C2951">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/984/1.png", 2)</f>
@@ -23331,7 +23368,7 @@
         <v>985</v>
       </c>
       <c r="B2954" s="3" t="s">
-        <v>1001</v>
+        <v>1005</v>
       </c>
       <c r="C2954">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/985/1.png", 2)</f>
@@ -23351,7 +23388,7 @@
         <v>986</v>
       </c>
       <c r="B2957" s="3" t="s">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="C2957">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/986/1.png", 2)</f>
@@ -23371,7 +23408,7 @@
         <v>987</v>
       </c>
       <c r="B2960" s="3" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
       <c r="C2960">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/987/1.png", 2)</f>
@@ -23391,7 +23428,7 @@
         <v>988</v>
       </c>
       <c r="B2963" s="3" t="s">
-        <v>1004</v>
+        <v>1008</v>
       </c>
       <c r="C2963">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/988/1.png", 2)</f>
@@ -23411,7 +23448,7 @@
         <v>989</v>
       </c>
       <c r="B2966" s="3" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="C2966">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/989/1.png", 2)</f>
@@ -23431,7 +23468,7 @@
         <v>990</v>
       </c>
       <c r="B2969" s="3" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="C2969">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/990/1.png", 2)</f>
@@ -23451,7 +23488,7 @@
         <v>991</v>
       </c>
       <c r="B2972" s="3" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="C2972">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/991/1.png", 2)</f>
@@ -23471,7 +23508,7 @@
         <v>992</v>
       </c>
       <c r="B2975" s="3" t="s">
-        <v>1008</v>
+        <v>1012</v>
       </c>
       <c r="C2975">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/992/1.png", 2)</f>
@@ -23491,7 +23528,7 @@
         <v>993</v>
       </c>
       <c r="B2978" s="3" t="s">
-        <v>1009</v>
+        <v>1013</v>
       </c>
       <c r="C2978">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/993/1.png", 2)</f>
@@ -23511,7 +23548,7 @@
         <v>994</v>
       </c>
       <c r="B2981" s="3" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="C2981">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/994/1.png", 2)</f>
@@ -23531,7 +23568,7 @@
         <v>995</v>
       </c>
       <c r="B2984" s="3" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="C2984">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/995/1.png", 2)</f>
@@ -23551,7 +23588,7 @@
         <v>996</v>
       </c>
       <c r="B2987" s="3" t="s">
-        <v>1012</v>
+        <v>1016</v>
       </c>
       <c r="C2987">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/996/1.png", 2)</f>
@@ -23571,7 +23608,7 @@
         <v>997</v>
       </c>
       <c r="B2990" s="3" t="s">
-        <v>1013</v>
+        <v>1017</v>
       </c>
       <c r="C2990">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/997/1.png", 2)</f>
@@ -23591,7 +23628,7 @@
         <v>998</v>
       </c>
       <c r="B2993" s="3" t="s">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="C2993">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/998/1.png", 2)</f>
@@ -23611,7 +23648,7 @@
         <v>999</v>
       </c>
       <c r="B2996" s="3" t="s">
-        <v>1015</v>
+        <v>1019</v>
       </c>
       <c r="C2996">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/999/1.png", 2)</f>
@@ -23631,7 +23668,7 @@
         <v>1000</v>
       </c>
       <c r="B2999" s="3" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="C2999">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1000/1.png", 2)</f>
@@ -23651,7 +23688,7 @@
         <v>1001</v>
       </c>
       <c r="B3002" s="3" t="s">
-        <v>1017</v>
+        <v>1021</v>
       </c>
       <c r="C3002">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1001/1.png", 2)</f>
@@ -23671,7 +23708,7 @@
         <v>1002</v>
       </c>
       <c r="B3005" s="3" t="s">
-        <v>1018</v>
+        <v>1022</v>
       </c>
       <c r="C3005">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1002/1.png", 2)</f>
@@ -23691,7 +23728,7 @@
         <v>1003</v>
       </c>
       <c r="B3008" s="3" t="s">
-        <v>1019</v>
+        <v>1023</v>
       </c>
       <c r="C3008">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1003/1.png", 2)</f>
@@ -23711,7 +23748,7 @@
         <v>1004</v>
       </c>
       <c r="B3011" s="3" t="s">
-        <v>1020</v>
+        <v>1024</v>
       </c>
       <c r="C3011">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1004/1.png", 2)</f>
@@ -23731,7 +23768,7 @@
         <v>1005</v>
       </c>
       <c r="B3014" s="3" t="s">
-        <v>1021</v>
+        <v>1025</v>
       </c>
       <c r="C3014">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1005/1.png", 2)</f>
@@ -23751,7 +23788,7 @@
         <v>1006</v>
       </c>
       <c r="B3017" s="3" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="C3017">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1006/1.png", 2)</f>
@@ -23771,7 +23808,7 @@
         <v>1007</v>
       </c>
       <c r="B3020" s="3" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
       <c r="C3020">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1007/1.png", 2)</f>
@@ -23791,7 +23828,7 @@
         <v>1008</v>
       </c>
       <c r="B3023" s="3" t="s">
-        <v>1024</v>
+        <v>1028</v>
       </c>
       <c r="C3023">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1008/1.png", 2)</f>
@@ -23811,7 +23848,7 @@
         <v>1009</v>
       </c>
       <c r="B3026" s="3" t="s">
-        <v>1025</v>
+        <v>1029</v>
       </c>
       <c r="C3026">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1009/1.png", 2)</f>
@@ -23831,7 +23868,7 @@
         <v>1010</v>
       </c>
       <c r="B3029" s="3" t="s">
-        <v>1026</v>
+        <v>1030</v>
       </c>
       <c r="C3029">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1010/1.png", 2)</f>
@@ -23851,7 +23888,7 @@
         <v>1011</v>
       </c>
       <c r="B3032" s="3" t="s">
-        <v>1027</v>
+        <v>1031</v>
       </c>
       <c r="C3032">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1011/1.png", 2)</f>
@@ -23871,7 +23908,7 @@
         <v>1012</v>
       </c>
       <c r="B3035" s="3" t="s">
-        <v>1028</v>
+        <v>1032</v>
       </c>
       <c r="C3035">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1012/1.png", 2)</f>
@@ -23891,7 +23928,7 @@
         <v>1013</v>
       </c>
       <c r="B3038" s="3" t="s">
-        <v>1029</v>
+        <v>1033</v>
       </c>
       <c r="C3038">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1013/1.png", 2)</f>
@@ -23911,7 +23948,7 @@
         <v>1014</v>
       </c>
       <c r="B3041" s="3" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c r="C3041">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1014/1.png", 2)</f>
@@ -23931,7 +23968,7 @@
         <v>1015</v>
       </c>
       <c r="B3044" s="3" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
       <c r="C3044">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1015/1.png", 2)</f>
@@ -23951,7 +23988,7 @@
         <v>1016</v>
       </c>
       <c r="B3047" s="3" t="s">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c r="C3047">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1016/1.png", 2)</f>
@@ -23971,7 +24008,7 @@
         <v>1017</v>
       </c>
       <c r="B3050" s="3" t="s">
-        <v>1033</v>
+        <v>1037</v>
       </c>
       <c r="C3050">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1017/1.png", 2)</f>
@@ -23991,7 +24028,7 @@
         <v>1018</v>
       </c>
       <c r="B3053" s="3" t="s">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="C3053">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1018/1.png", 2)</f>
@@ -24011,7 +24048,7 @@
         <v>1019</v>
       </c>
       <c r="B3056" s="3" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
       <c r="C3056">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1019/1.png", 2)</f>
@@ -24031,7 +24068,7 @@
         <v>1020</v>
       </c>
       <c r="B3059" s="3" t="s">
-        <v>1036</v>
+        <v>1040</v>
       </c>
       <c r="C3059">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1020/1.png", 2)</f>
@@ -24051,7 +24088,7 @@
         <v>1021</v>
       </c>
       <c r="B3062" s="3" t="s">
-        <v>1037</v>
+        <v>1041</v>
       </c>
       <c r="C3062">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1021/1.png", 2)</f>
@@ -24071,7 +24108,7 @@
         <v>1022</v>
       </c>
       <c r="B3065" s="3" t="s">
-        <v>1038</v>
+        <v>1042</v>
       </c>
       <c r="C3065">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1022/1.png", 2)</f>
@@ -24091,7 +24128,7 @@
         <v>1023</v>
       </c>
       <c r="B3068" s="3" t="s">
-        <v>1039</v>
+        <v>1043</v>
       </c>
       <c r="C3068">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1023/1.png", 2)</f>
@@ -24111,7 +24148,7 @@
         <v>1024</v>
       </c>
       <c r="B3071" s="3" t="s">
-        <v>1040</v>
+        <v>1044</v>
       </c>
       <c r="C3071">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1024/1.png", 2)</f>
@@ -24131,7 +24168,7 @@
         <v>1025</v>
       </c>
       <c r="B3074" s="3" t="s">
-        <v>1041</v>
+        <v>1045</v>
       </c>
       <c r="C3074">
         <f>IMAGE("https://raw.githubusercontent.com/stautonico/tcg-livingdex/main/images/1025/1.png", 2)</f>

</xml_diff>